<commit_message>
Fix path for linked tables. Fix error recovery code. Fix household_members form (bad column name - values_list)
</commit_message>
<xml_diff>
--- a/form-files/tables/household_member/forms/household_member/household_member.xlsx
+++ b/form-files/tables/household_member/forms/household_member/household_member.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="3144" windowWidth="23652" windowHeight="18240" activeTab="2"/>
+    <workbookView xWindow="290" yWindow="3140" windowWidth="23650" windowHeight="16220"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>display.image</t>
   </si>
   <si>
-    <t>value_list</t>
-  </si>
-  <si>
     <t>select_one</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>survey</t>
+  </si>
+  <si>
+    <t>values_list</t>
   </si>
 </sst>
 </file>
@@ -578,26 +578,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="41.90625" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -606,7 +606,7 @@
         <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
         <v>31</v>
@@ -615,7 +615,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="36.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -634,7 +634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -647,7 +647,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -658,9 +658,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -672,9 +672,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -686,7 +686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="40.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -698,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -710,7 +710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" ht="34.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -737,14 +737,14 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="1" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -758,7 +758,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -769,7 +769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -780,8 +780,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="5" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -792,7 +792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -812,18 +812,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
@@ -831,10 +831,10 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -842,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -850,7 +850,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>36</v>
       </c>
@@ -858,9 +858,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
@@ -880,16 +880,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="46.109375" customWidth="1"/>
+    <col min="5" max="5" width="46.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -897,16 +897,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
       </c>
       <c r="E1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="132.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="132.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -923,8 +923,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="4" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="1:5" ht="12.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" ht="12.65" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update handlebarHelpers and create usage examples in household_member. Move copy.bat up to copy FORM and XLSX as one step.
</commit_message>
<xml_diff>
--- a/form-files/tables/household_member/forms/household_member/household_member.xlsx
+++ b/form-files/tables/household_member/forms/household_member/household_member.xlsx
@@ -11,13 +11,14 @@
     <sheet name="choices" sheetId="3" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
     <sheet name="model" sheetId="5" r:id="rId4"/>
+    <sheet name="calculates" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>type</t>
   </si>
@@ -61,16 +62,7 @@
     <t>age</t>
   </si>
   <si>
-    <t>Enter age:</t>
-  </si>
-  <si>
-    <t>Enter sex:</t>
-  </si>
-  <si>
     <t>sex</t>
-  </si>
-  <si>
-    <t>Does this household member contribute to the household income?</t>
   </si>
   <si>
     <t>household_member</t>
@@ -207,6 +199,33 @@
   </si>
   <si>
     <t>values_list</t>
+  </si>
+  <si>
+    <t>Enter age of {{member_name}}:</t>
+  </si>
+  <si>
+    <t>Enter sex of {{member_name}}:</t>
+  </si>
+  <si>
+    <t>Does {{member_name}} contribute to the household income?</t>
+  </si>
+  <si>
+    <t>calculation_name</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>ageIsOddOrEven</t>
+  </si>
+  <si>
+    <t>((data('age') % 2) == 1) ? "odd" : "even"</t>
+  </si>
+  <si>
+    <t>{{member_name}} age is {{evaluate calculates.ageIsOddOrEven}} in {{setting 'table_id'}} for {{metadata 'instanceName'}}</t>
   </si>
 </sst>
 </file>
@@ -576,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -597,22 +616,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="36.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -621,17 +640,17 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -640,10 +659,10 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -655,74 +674,82 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="40.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
       <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="40.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="34.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -734,7 +761,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -746,16 +773,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -825,13 +852,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -839,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,19 +879,19 @@
     </row>
     <row r="4" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -897,30 +924,30 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="132.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.65" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -929,4 +956,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="44.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change the household id in the household members form to be a note (not editable)
</commit_message>
<xml_diff>
--- a/form-files/tables/household_member/forms/household_member/household_member.xlsx
+++ b/form-files/tables/household_member/forms/household_member/household_member.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="3140" windowWidth="23660" windowHeight="16220"/>
+    <workbookView xWindow="300" yWindow="3140" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>type</t>
   </si>
@@ -109,16 +109,7 @@
     <t>household_id</t>
   </si>
   <si>
-    <t>readonly</t>
-  </si>
-  <si>
     <t>comments</t>
-  </si>
-  <si>
-    <t>readonly is not implemented, but this would be a note-like field that was set to be the parent table key via the extra URL arguments.  It could be hidden and only displayed as a reference in a prompt label.</t>
-  </si>
-  <si>
-    <t>Unique barcode ID or locator designation for this household (foreign key into household table).</t>
   </si>
   <si>
     <t>string</t>
@@ -237,6 +228,9 @@
   </si>
   <si>
     <t>hideInContents</t>
+  </si>
+  <si>
+    <t>Data for household: {{household_id}}</t>
   </si>
 </sst>
 </file>
@@ -606,69 +600,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="41.81640625" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="36.75" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1">
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -681,7 +660,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -689,12 +668,12 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -703,23 +682,23 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="62.5" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="62.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="b">
+      <c r="F6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="42" customHeight="1">
+    <row r="7" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -728,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="40.75" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="40.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -743,7 +722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="35.5" customHeight="1">
+    <row r="9" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -755,7 +734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="34.25" customHeight="1">
+    <row r="10" spans="1:6" ht="34.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -767,7 +746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1"/>
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -787,28 +766,28 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="1" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.25" customHeight="1">
+    <row r="1" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="22.25" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -819,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.25" customHeight="1">
+    <row r="3" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -830,8 +809,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22.25" customHeight="1"/>
-    <row r="5" spans="1:4" ht="22.25" customHeight="1">
+    <row r="4" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -842,7 +821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22.25" customHeight="1">
+    <row r="6" spans="1:4" ht="22.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -871,25 +850,25 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -897,7 +876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -905,26 +884,26 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.75" customHeight="1">
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -948,16 +927,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="46.1640625" customWidth="1"/>
+    <col min="5" max="5" width="46.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.5" customHeight="1">
+    <row r="1" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -965,21 +944,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="132.75" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -988,11 +967,11 @@
         <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1"/>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1012,26 +991,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="44.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" customHeight="1">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>